<commit_message>
Erica adds phenology data ground truthing
</commit_message>
<xml_diff>
--- a/data/phenology/groundtruthing_2022/phenocam_groundtruthing_common_garden22_copy5.xlsx
+++ b/data/phenology/groundtruthing_2022/phenocam_groundtruthing_common_garden22_copy5.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericazaja/Desktop/Github_repos.tmp/GardenHub/data/phenology/groundtruthing_2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0048422-8B9C-9742-B518-0F1EEF3ADE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBA2FF-07C5-704F-9DC6-1E9CDFC31838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="500" windowWidth="24640" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -511,29 +511,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -760,7 +758,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -834,1139 +832,1103 @@
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>44745</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="6">
         <v>44732</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6">
         <v>44743</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>44745</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="7">
         <v>44732</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>44752</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>44752</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>44732</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>44745</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="J6" s="8">
+      <c r="J6" s="6">
         <v>44745</v>
       </c>
-      <c r="K6" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L6" s="13">
-        <v>44785</v>
-      </c>
-      <c r="M6" s="7" t="s">
+      <c r="K6" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L6" s="11">
+        <v>44785</v>
+      </c>
+      <c r="M6" t="s">
         <v>37</v>
       </c>
-      <c r="R6" s="12" t="s">
+      <c r="R6" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="7" t="s">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="J7" s="8">
+      <c r="J7" s="6">
         <v>44745</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="M7" s="7" t="s">
+      <c r="K7" s="8"/>
+      <c r="M7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="J8" s="8">
+      <c r="J8" s="6">
         <v>44752</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>44765</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="M8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="J9" s="8">
+      <c r="J9" s="6">
         <v>44745</v>
       </c>
-      <c r="K9" s="14">
+      <c r="K9" s="12">
         <v>44841</v>
       </c>
-      <c r="L9" s="13">
-        <v>44785</v>
-      </c>
-      <c r="M9" s="7" t="s">
+      <c r="L9" s="11">
+        <v>44785</v>
+      </c>
+      <c r="M9" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="J10" s="8">
+      <c r="J10" s="6">
         <v>44752</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13">
-        <v>44785</v>
-      </c>
-      <c r="M10" s="7" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="11">
+        <v>44785</v>
+      </c>
+      <c r="M10" t="s">
         <v>46</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" t="s">
         <v>47</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="J11" s="8">
+      <c r="J11" s="6">
         <v>44752</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="K11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+      <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L12" s="13">
+      <c r="K12" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L12" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
+      <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="J13" s="8">
+      <c r="J13" s="6">
         <v>44745</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="J14" s="8">
+      <c r="J14" s="6">
         <v>44745</v>
       </c>
-      <c r="K14" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L14" s="13">
+      <c r="K14" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L14" s="11">
         <v>44765</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="12" t="s">
+      <c r="R14" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L15" s="13">
+      <c r="K15" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L15" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="7" t="s">
+      <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="K16" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="R16" s="12" t="s">
+      <c r="R16" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="J17" s="8">
+      <c r="J17" s="6">
         <v>44745</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="12">
         <v>44841</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="11">
         <v>44765</v>
       </c>
-      <c r="M17" s="7" t="s">
+      <c r="M17" t="s">
         <v>59</v>
       </c>
-      <c r="N17" s="7" t="s">
+      <c r="N17" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="7" t="s">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="J18" s="8">
+      <c r="J18" s="6">
         <v>44745</v>
       </c>
-      <c r="K18" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L18" s="10" t="s">
+      <c r="K18" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="7" t="s">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="6">
         <v>44739</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="K20" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="7" t="s">
+      <c r="A21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L21" s="12" t="s">
+      <c r="K21" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L21" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="7" t="s">
+      <c r="A22" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="12" t="s">
+      <c r="K22" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K23" s="12" t="s">
+      <c r="K23" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="7" t="s">
+      <c r="A24" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="7" t="s">
+      <c r="A25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="J26" s="10" t="s">
+      <c r="J26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K26" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L26" s="13">
-        <v>44785</v>
-      </c>
-      <c r="R26" s="12" t="s">
+      <c r="K26" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L26" s="11">
+        <v>44785</v>
+      </c>
+      <c r="R26" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="7" t="s">
+      <c r="A27" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="7"/>
-      <c r="J27" s="10" t="s">
+      <c r="J27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="M27" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="7" t="s">
+      <c r="A28" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="7"/>
-      <c r="J28" s="10" t="s">
+      <c r="J28" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K28" s="15">
+      <c r="K28" s="13">
         <v>44732</v>
       </c>
-      <c r="M28" s="7" t="s">
+      <c r="M28" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" t="s">
         <v>80</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="6">
         <v>44745</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="6">
         <v>44739</v>
       </c>
-      <c r="J29" s="8">
+      <c r="J29" s="6">
         <v>44745</v>
       </c>
-      <c r="M29" s="7" t="s">
+      <c r="M29" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="7" t="s">
+      <c r="A30" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="8">
+      <c r="G30" s="6">
         <v>44745</v>
       </c>
-      <c r="H30" s="8">
+      <c r="H30" s="6">
         <v>44739</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="6">
         <v>44752</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="11">
         <v>44765</v>
       </c>
-      <c r="M30" s="7" t="s">
+      <c r="M30" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
+      <c r="A31" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="J32" s="8">
+      <c r="J32" s="6">
         <v>44752</v>
       </c>
-      <c r="K32" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L32" s="13">
+      <c r="K32" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L32" s="11">
         <v>44765</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="7" t="s">
+      <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" t="s">
         <v>66</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="J33" s="10" t="s">
+      <c r="J33" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K33" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L33" s="13">
+      <c r="K33" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L33" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="7" t="s">
+      <c r="A34" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="J34" s="10" t="s">
+      <c r="J34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K34" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L34" s="13">
+      <c r="K34" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L34" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" t="s">
         <v>89</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6">
         <v>44739</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="6">
         <v>44745</v>
       </c>
-      <c r="J35" s="10" t="s">
+      <c r="J35" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="7" t="s">
+      <c r="A36" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" t="s">
         <v>90</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="J36" s="10" t="s">
+      <c r="J36" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K36" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L36" s="12" t="s">
+      <c r="K36" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L36" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="M36" s="10" t="s">
+      <c r="M36" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="R36" s="12" t="s">
+      <c r="R36" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="7" t="s">
+      <c r="A37" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="J37" s="10" t="s">
+      <c r="J37" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K37" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L37" s="10" t="s">
+      <c r="K37" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L37" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="7"/>
-      <c r="J38" s="10" t="s">
+      <c r="J38" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="7" t="s">
+      <c r="A39" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="J39" s="10" t="s">
+      <c r="J39" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K39" s="13">
+      <c r="K39" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="7" t="s">
+      <c r="A40" t="s">
         <v>93</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="7"/>
-      <c r="J40" s="10" t="s">
+      <c r="J40" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K40" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L40" s="13">
-        <v>44785</v>
-      </c>
-      <c r="N40" s="7" t="s">
+      <c r="K40" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L40" s="11">
+        <v>44785</v>
+      </c>
+      <c r="N40" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="J41" s="8">
+      <c r="J41" s="6">
         <v>44745</v>
       </c>
-      <c r="K41" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L41" s="13">
+      <c r="K41" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L41" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="7" t="s">
+      <c r="A42" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" t="s">
         <v>100</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="J42" s="10" t="s">
+      <c r="J42" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K42" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L42" s="13">
+      <c r="K42" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L42" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="7" t="s">
+      <c r="A43" t="s">
         <v>98</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="J43" s="8">
+      <c r="J43" s="6">
         <v>44745</v>
       </c>
-      <c r="K43" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L43" s="13">
+      <c r="K43" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L43" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" t="s">
         <v>66</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="J44" s="8">
+      <c r="J44" s="6">
         <v>44739</v>
       </c>
-      <c r="K44" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L44" s="13">
-        <v>44785</v>
-      </c>
-      <c r="M44" s="7" t="s">
+      <c r="K44" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L44" s="11">
+        <v>44785</v>
+      </c>
+      <c r="M44" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="7" t="s">
+      <c r="A45" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="J45" s="10" t="s">
+      <c r="J45" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K45" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L45" s="13">
+      <c r="K45" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L45" s="11">
         <v>44785</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="7" t="s">
+      <c r="A46" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="7"/>
-      <c r="J46" s="10" t="s">
+      <c r="J46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="K46" s="13">
-        <v>44785</v>
-      </c>
-      <c r="L46" s="13">
+      <c r="K46" s="11">
+        <v>44785</v>
+      </c>
+      <c r="L46" s="11">
         <v>44785</v>
       </c>
     </row>
@@ -1981,7 +1943,7 @@
     <row r="55" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="56" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="57" spans="12:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="L57" s="13">
+      <c r="L57" s="11">
         <v>44785</v>
       </c>
     </row>
@@ -2193,13 +2155,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$1:$A$3</xm:f>
+            <xm:f>instructions!$A$1:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$5:$A$6</xm:f>
+            <xm:f>instructions!$A$5:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E46</xm:sqref>
         </x14:dataValidation>
@@ -2227,95 +2189,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="7" t="s">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="7" t="s">
+      <c r="A6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="15" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>